<commit_message>
Update requirements file & ReadMe file
</commit_message>
<xml_diff>
--- a/input/comp_mrs_db_dog.xlsx
+++ b/input/comp_mrs_db_dog.xlsx
@@ -2310,7 +2310,7 @@
         <v>0.1539807218308993</v>
       </c>
       <c r="AK15" t="n">
-        <v>-0.2442516445297177</v>
+        <v>-0.2361937233542203</v>
       </c>
       <c r="AL15" t="n">
         <v>-8.451166396474795</v>
@@ -2552,7 +2552,7 @@
         <v>0.2962130218452153</v>
       </c>
       <c r="AK17" t="n">
-        <v>0.8760989568824644</v>
+        <v>0.9087642915481414</v>
       </c>
       <c r="AL17" t="n">
         <v>-7.257492808936883</v>
@@ -2915,7 +2915,7 @@
         <v>-0.09412395573830512</v>
       </c>
       <c r="AK20" t="n">
-        <v>-0.1702074627298488</v>
+        <v>-0.1674598846420003</v>
       </c>
       <c r="AL20" t="n">
         <v>-11.14960785993486</v>
@@ -3278,7 +3278,7 @@
         <v>0.2036595958697739</v>
       </c>
       <c r="AK23" t="n">
-        <v>0.0006344048952334065</v>
+        <v>0.198583478680728</v>
       </c>
       <c r="AL23" t="n">
         <v>-13.12398390372212</v>
@@ -4730,7 +4730,7 @@
         <v>0.3488921036616279</v>
       </c>
       <c r="AK35" t="n">
-        <v>1.043570263957005</v>
+        <v>1.045020814677251</v>
       </c>
       <c r="AL35" t="n">
         <v>-9.029699704606241</v>
@@ -6182,7 +6182,7 @@
         <v>-0.02000160997978494</v>
       </c>
       <c r="AK47" t="n">
-        <v>-0.3513754254930812</v>
+        <v>0.3723286718929898</v>
       </c>
       <c r="AL47" t="n">
         <v>-6.722520401440502</v>
@@ -6666,7 +6666,7 @@
         <v>0.1560580424000802</v>
       </c>
       <c r="AK51" t="n">
-        <v>0.003887327139737095</v>
+        <v>0.0064879006702625</v>
       </c>
       <c r="AL51" t="n">
         <v>-11.44397767834532</v>
@@ -6787,7 +6787,7 @@
         <v>-0.2077082796478813</v>
       </c>
       <c r="AK52" t="n">
-        <v>-0.8199392948410563</v>
+        <v>-0.8161424923930423</v>
       </c>
       <c r="AL52" t="n">
         <v>-12.57711222015901</v>
@@ -6908,7 +6908,7 @@
         <v>0.2569478745805414</v>
       </c>
       <c r="AK53" t="n">
-        <v>-0.1849290071183466</v>
+        <v>-0.1819545794796578</v>
       </c>
       <c r="AL53" t="n">
         <v>-8.079684942188528</v>
@@ -7029,7 +7029,7 @@
         <v>0.1816933742245348</v>
       </c>
       <c r="AK54" t="n">
-        <v>-0.00330345636574594</v>
+        <v>0.0001117657469750415</v>
       </c>
       <c r="AL54" t="n">
         <v>-11.2134410767811</v>
@@ -7392,7 +7392,7 @@
         <v>0.1752452879725516</v>
       </c>
       <c r="AK57" t="n">
-        <v>0.1231134291798312</v>
+        <v>0.1248089669073825</v>
       </c>
       <c r="AL57" t="n">
         <v>-7.644414549991064</v>
@@ -7634,7 +7634,7 @@
         <v>0.0001785114789394253</v>
       </c>
       <c r="AK59" t="n">
-        <v>-3.080117332062254</v>
+        <v>-3.074226453257253</v>
       </c>
       <c r="AL59" t="n">
         <v>-11.40970585399761</v>
@@ -8965,7 +8965,7 @@
         <v>0.0563064883312854</v>
       </c>
       <c r="AK70" t="n">
-        <v>0.1105711794503023</v>
+        <v>0.1247704875268558</v>
       </c>
       <c r="AL70" t="n">
         <v>-8.88233198388316</v>
@@ -9328,7 +9328,7 @@
         <v>0.03135610442776928</v>
       </c>
       <c r="AK73" t="n">
-        <v>0.01166214964743761</v>
+        <v>0.08545147540766225</v>
       </c>
       <c r="AL73" t="n">
         <v>-11.93633320006451</v>
@@ -9812,7 +9812,7 @@
         <v>0.1641204189601657</v>
       </c>
       <c r="AK77" t="n">
-        <v>0.6081348643132892</v>
+        <v>0.6220035124417286</v>
       </c>
       <c r="AL77" t="n">
         <v>-7.73280622254592</v>
@@ -10175,7 +10175,7 @@
         <v>0.05139794557285706</v>
       </c>
       <c r="AK80" t="n">
-        <v>0.01756079226143276</v>
+        <v>0.02265103433439437</v>
       </c>
       <c r="AL80" t="n">
         <v>-11.40993644727429</v>
@@ -10417,7 +10417,7 @@
         <v>-0.03223518003632108</v>
       </c>
       <c r="AK82" t="n">
-        <v>-0.07779048644755447</v>
+        <v>-0.07565457262621215</v>
       </c>
       <c r="AL82" t="n">
         <v>-9.437435407552986</v>
@@ -10780,7 +10780,7 @@
         <v>-0.05112431594338047</v>
       </c>
       <c r="AK85" t="n">
-        <v>-0.7647301797721917</v>
+        <v>-0.7481499317802403</v>
       </c>
       <c r="AL85" t="n">
         <v>-9.711890026635315</v>
@@ -11385,7 +11385,7 @@
         <v>0.2306404980166452</v>
       </c>
       <c r="AK90" t="n">
-        <v>0.7432234474006838</v>
+        <v>0.7459726778380995</v>
       </c>
       <c r="AL90" t="n">
         <v>-5.614459330744943</v>
@@ -11748,7 +11748,7 @@
         <v>0.2608321684737274</v>
       </c>
       <c r="AK93" t="n">
-        <v>0.5049059281702621</v>
+        <v>0.5087229195352737</v>
       </c>
       <c r="AL93" t="n">
         <v>-5.873510411949113</v>
@@ -13805,7 +13805,7 @@
         <v>-0.0077995536038212</v>
       </c>
       <c r="AK110" t="n">
-        <v>-0.8083417276770196</v>
+        <v>-0.804601333512558</v>
       </c>
       <c r="AL110" t="n">
         <v>-11.3857516698281</v>
@@ -13926,7 +13926,7 @@
         <v>-0.0849532940945425</v>
       </c>
       <c r="AK111" t="n">
-        <v>-1.796775905961965</v>
+        <v>-1.685359506564677</v>
       </c>
       <c r="AL111" t="n">
         <v>-10.02555049525445</v>
@@ -14410,7 +14410,7 @@
         <v>0.2140602774625162</v>
       </c>
       <c r="AK115" t="n">
-        <v>0.1676729881882217</v>
+        <v>0.1739777147364865</v>
       </c>
       <c r="AL115" t="n">
         <v>-9.037867117110411</v>
@@ -14894,7 +14894,7 @@
         <v>-0.0007541660549133119</v>
       </c>
       <c r="AK119" t="n">
-        <v>-0.3078273142744736</v>
+        <v>0.04039942665221888</v>
       </c>
       <c r="AL119" t="n">
         <v>-9.633210722718722</v>
@@ -15499,7 +15499,7 @@
         <v>0.1316139940554002</v>
       </c>
       <c r="AK124" t="n">
-        <v>0.008083704509054719</v>
+        <v>0.0101069761950409</v>
       </c>
       <c r="AL124" t="n">
         <v>-10.68605617810361</v>
@@ -15862,7 +15862,7 @@
         <v>0.2778761717435449</v>
       </c>
       <c r="AK127" t="n">
-        <v>-0.3069045578505933</v>
+        <v>-0.3054881633986597</v>
       </c>
       <c r="AL127" t="n">
         <v>-13.24470743249028</v>
@@ -16225,7 +16225,7 @@
         <v>0.01253370692536285</v>
       </c>
       <c r="AK130" t="n">
-        <v>0.3147184981613569</v>
+        <v>0.3167004954033975</v>
       </c>
       <c r="AL130" t="n">
         <v>-9.326523330763616</v>
@@ -16467,7 +16467,7 @@
         <v>0.2243305446669307</v>
       </c>
       <c r="AK132" t="n">
-        <v>-0.02673093086952361</v>
+        <v>-0.02505799165947572</v>
       </c>
       <c r="AL132" t="n">
         <v>-7.439336016482929</v>
@@ -16709,7 +16709,7 @@
         <v>0.2811669469844215</v>
       </c>
       <c r="AK134" t="n">
-        <v>0.3928838871229469</v>
+        <v>0.3956965028851673</v>
       </c>
       <c r="AL134" t="n">
         <v>-7.833305169472409</v>
@@ -16830,7 +16830,7 @@
         <v>-0.1395954448533699</v>
       </c>
       <c r="AK135" t="n">
-        <v>-0.3023880219403225</v>
+        <v>-0.3000403515826187</v>
       </c>
       <c r="AL135" t="n">
         <v>-10.88021305327009</v>
@@ -17072,7 +17072,7 @@
         <v>0.004627323146514133</v>
       </c>
       <c r="AK137" t="n">
-        <v>0.4140787321128346</v>
+        <v>0.8218868871898892</v>
       </c>
       <c r="AL137" t="n">
         <v>-10.28094554376941</v>
@@ -17798,7 +17798,7 @@
         <v>0.04795996658599886</v>
       </c>
       <c r="AK143" t="n">
-        <v>-0.7717199703195817</v>
+        <v>-0.6909274509321809</v>
       </c>
       <c r="AL143" t="n">
         <v>-9.144541282086077</v>
@@ -18161,7 +18161,7 @@
         <v>0.1467939995270025</v>
       </c>
       <c r="AK146" t="n">
-        <v>0.06436714771638037</v>
+        <v>0.06806910517548249</v>
       </c>
       <c r="AL146" t="n">
         <v>-9.929866801649126</v>
@@ -18403,7 +18403,7 @@
         <v>0.02553700368941194</v>
       </c>
       <c r="AK148" t="n">
-        <v>0.7700781547136075</v>
+        <v>0.7734460882229646</v>
       </c>
       <c r="AL148" t="n">
         <v>-8.743028378214424</v>
@@ -18887,7 +18887,7 @@
         <v>0.2257968305255448</v>
       </c>
       <c r="AK152" t="n">
-        <v>0.7242162743359597</v>
+        <v>0.7262242046865546</v>
       </c>
       <c r="AL152" t="n">
         <v>-10.50896334152284</v>
@@ -19250,7 +19250,7 @@
         <v>0.2160151335558353</v>
       </c>
       <c r="AK155" t="n">
-        <v>0.1924262620971286</v>
+        <v>0.2023313492158028</v>
       </c>
       <c r="AL155" t="n">
         <v>-9.191514744549854</v>
@@ -19492,7 +19492,7 @@
         <v>-0.05252915257097401</v>
       </c>
       <c r="AK157" t="n">
-        <v>-0.944200788308289</v>
+        <v>-0.9416178469376432</v>
       </c>
       <c r="AL157" t="n">
         <v>-10.43427905361962</v>
@@ -20460,7 +20460,7 @@
         <v>0.2534432936141042</v>
       </c>
       <c r="AK165" t="n">
-        <v>0.05916469469561396</v>
+        <v>0.06671454987488046</v>
       </c>
       <c r="AL165" t="n">
         <v>-8.912998047912499</v>
@@ -20581,7 +20581,7 @@
         <v>0.2591291549157473</v>
       </c>
       <c r="AK166" t="n">
-        <v>0.8670662807905248</v>
+        <v>0.8872597965282166</v>
       </c>
       <c r="AL166" t="n">
         <v>-9.642205030561344</v>
@@ -20702,7 +20702,7 @@
         <v>0.05074028835899175</v>
       </c>
       <c r="AK167" t="n">
-        <v>1.212061784103416</v>
+        <v>1.515368923590123</v>
       </c>
       <c r="AL167" t="n">
         <v>-8.295054975684208</v>
@@ -20823,7 +20823,7 @@
         <v>-0.1468047655011192</v>
       </c>
       <c r="AK168" t="n">
-        <v>-1.186252107208071</v>
+        <v>-1.160969573976397</v>
       </c>
       <c r="AL168" t="n">
         <v>-10.76958255958851</v>
@@ -20944,7 +20944,7 @@
         <v>0.03559215304512069</v>
       </c>
       <c r="AK169" t="n">
-        <v>-0.1145011618341881</v>
+        <v>-0.1123810966921291</v>
       </c>
       <c r="AL169" t="n">
         <v>-9.609318240946729</v>
@@ -21065,7 +21065,7 @@
         <v>-0.04612204868726691</v>
       </c>
       <c r="AK170" t="n">
-        <v>0.13960191438372</v>
+        <v>0.1462427124229041</v>
       </c>
       <c r="AL170" t="n">
         <v>-12.35643114738403</v>
@@ -21186,7 +21186,7 @@
         <v>0.1530485017959816</v>
       </c>
       <c r="AK171" t="n">
-        <v>0.3583320470313792</v>
+        <v>0.3634930641779162</v>
       </c>
       <c r="AL171" t="n">
         <v>-11.48594968308679</v>

</xml_diff>